<commit_message>
Updated notebook and reports
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada-coimbra.xlsx
+++ b/notebooks/jesuita-entrada-coimbra.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,37 +446,42 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>nascimento.date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>jesuita-entrada.date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>jesuita-entrada</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>jesuita-entrada.type</t>
-        </is>
-      </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>nascimento.date</t>
+          <t>age_at_entrada</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>tempo_em_coimbra</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>embarque</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>embarque.date</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>embarque.obs</t>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>age_at_embarque</t>
         </is>
       </c>
     </row>
@@ -493,35 +498,38 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>16170000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>16350000</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>16170000</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>16430330</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -536,35 +544,38 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>16300000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>16490000</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>16300000</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>19</v>
+      </c>
+      <c r="G3" t="n">
+        <v>7</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Bom Jesus da Vidigueira</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>16570404</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -579,35 +590,38 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>16500000</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>16640325</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>16500000</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>13</v>
+      </c>
+      <c r="G4" t="n">
+        <v>31</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>[Para a China]</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>16940000</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -622,38 +636,37 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>16250000</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>16400000</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>16250000</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>15</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16</v>
+      </c>
+      <c r="H5" t="inlineStr">
         <is>
           <t>Bom Jesus da Vidigueira</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>16570404</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>extra_info: {"value": {"comment": "segundo Wicky"}}</t>
-        </is>
+      <c r="J5" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="6">
@@ -669,35 +682,38 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>15690000</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>15840114</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>15690000</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>14</v>
+      </c>
+      <c r="G6" t="n">
+        <v>33</v>
+      </c>
+      <c r="H6" t="inlineStr">
         <is>
           <t>Nossa Senhora da Guia</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>16170421</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -712,38 +728,37 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>16741102</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>16930310</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>16741102</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>16940000</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>extra_info: {"date": {"comment": "era novi\u00e7o"}}</t>
-        </is>
+      <c r="J7" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -759,160 +774,176 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>16540113</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>16690319</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>16540113</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>15</v>
+      </c>
+      <c r="G8" t="n">
+        <v>25</v>
+      </c>
+      <c r="H8" t="inlineStr">
         <is>
           <t>[Para a China]</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>16940000</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-abreu-ref1</t>
+          <t>deh-antonio-de-andrade</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>António de Abreu</t>
+          <t>António de Andrade</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>15760000</t>
+          <t>15800000</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15961216</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>15610000</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>16</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>S. Valentim</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>16000404</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-andrade</t>
+          <t>deh-antonio-de-gouvea</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>António de Andrade</t>
+          <t>António de Gouvea</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>15961216</t>
+          <t>15920000</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16080502</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>15800000</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>S. Valentim</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" t="n">
+        <v>15</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>16000404</t>
+          <t>[Para a Índia]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16230324</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-gouvea</t>
+          <t>deh-antonio-de-magalhaes</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>António de Gouvea</t>
+          <t>António de Magalhães</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16080502</t>
+          <t>16770000</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16921019</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>15920000</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>[Para a Índia]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>15</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>16230324</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>16960000</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -927,1299 +958,1314 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>16770000</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>16921019</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>16770000</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>15</v>
+      </c>
+      <c r="G12" t="n">
+        <v>32</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>16960000</t>
+          <t>[Para a China]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>17250000</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-magalhaes</t>
+          <t>deh-antonio-de-melo</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>António de Magalhães</t>
+          <t>António de Melo</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>16921019</t>
+          <t>16810803</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16990424</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>16770000</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>17</v>
+      </c>
+      <c r="G13" t="n">
+        <v>16</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>17250000</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr"/>
+          <t>S. Francisco Xavier</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>17150401</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-de-melo</t>
+          <t>deh-antonio-gomes</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>António de Melo</t>
+          <t>António Gomes</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16990424</t>
+          <t>17060000</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>17250528</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>16810803</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>S. Francisco Xavier</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>18</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>17150401</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>17270000</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-gomes</t>
+          <t>deh-antonio-lopes-junior</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>António Gomes</t>
+          <t>António Lopes, júnior</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>17250528</t>
+          <t>16690500</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16841225</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>17060000</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>11</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>17270000</t>
+          <t>[Para a China]</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "era novi\u00e7o"}}</t>
-        </is>
+          <t>16950000</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>deh-antonio-lopes-junior</t>
+          <t>deh-belchior-miguel-carneiro-leitao</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>António Lopes, júnior</t>
+          <t>Belchior Miguel Carneiro Leitão</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>16841225</t>
+          <t>15190000</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15430425</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>16690500</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>23</v>
+      </c>
+      <c r="G16" t="n">
+        <v>12</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>16950000</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr"/>
+          <t>S. Filipe</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>15550401</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>deh-belchior-miguel-carneiro-leitao</t>
+          <t>deh-belchior-nunes-barreto</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Belchior Miguel Carneiro Leitão</t>
+          <t>Belchior Nunes Barreto</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15430425</t>
+          <t>15190000</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15430311</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>15190000</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>S. Filipe</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>23</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>15550401</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+          <t>Esfera</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>15510310</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>deh-belchior-nunes-barreto</t>
+          <t>deh-cristovao-da-costa</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Belchior Nunes Barreto</t>
+          <t>Cristóvão da Costa</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15430311</t>
+          <t>15290000</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15500103</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>15190000</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Esfera</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>20</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
           <t>15510310</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>deh-cristovao-da-costa</t>
+          <t>deh-diogo-correia-valente</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cristóvão da Costa</t>
+          <t>Diogo Correia Valente</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>15500103</t>
+          <t>15680000</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15840110</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>15290000</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>15</v>
+      </c>
+      <c r="G19" t="n">
+        <v>34</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>15510310</t>
-        </is>
-      </c>
-      <c r="I19" t="inlineStr"/>
+          <t>Sto. Amaro</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>16180400</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>deh-diogo-correia-valente</t>
+          <t>deh-estanislau-machado</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Diogo Correia Valente</t>
+          <t>Estanislau Machado</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>15840110</t>
+          <t>16670000</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16810515</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>15680000</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Sto. Amaro</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>13</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>16180400</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "meados de Abril"}}</t>
-        </is>
+          <t>16870000</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>deh-estanislau-machado</t>
+          <t>deh-estevao-collasco</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Estanislau Machado</t>
+          <t>Estêvão Collasco</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16810515</t>
+          <t>16760421</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16920127</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>16670000</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>15</v>
+      </c>
+      <c r="G21" t="n">
+        <v>4</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>16870000</t>
+          <t>[Para a China]</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16950000</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>deh-estevao-collasco</t>
+          <t>deh-feliciano-da-silva</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Estêvão Collasco</t>
+          <t>Feliciano da Silva</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>16920127</t>
+          <t>15790000</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15931215</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>16760421</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>14</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>16950000</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16010411</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>deh-feliciano-da-silva</t>
+          <t>deh-francisco-furtado</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Feliciano da Silva</t>
+          <t>Francisco Furtado</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15931215</t>
+          <t>15890000</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16100000</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>15790000</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>20</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>16010411</t>
+          <t>S. Carlos</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16180400</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-furtado</t>
+          <t>deh-francisco-pacheco</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Francisco Furtado</t>
+          <t>Francisco Pacheco</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16100000</t>
+          <t>15680000</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15860000</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>15890000</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>S. Carlos</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>17</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>16180400</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "meio do m\u00eas"}}</t>
-        </is>
+          <t>15920407</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pacheco</t>
+          <t>deh-francisco-perez</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Francisco Pacheco</t>
+          <t>Francisco Pérez</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>15860000</t>
+          <t>15140000</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15440125</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>15680000</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>29</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>15920407</t>
+          <t>Flor de la Mar</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>15460408</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-perez</t>
+          <t>deh-francisco-pinto-i</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Francisco Pérez</t>
+          <t>Francisco Pinto</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>15440125</t>
+          <t>16620529</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16770527</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>15140000</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Flor de la Mar</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>14</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>15460408</t>
-        </is>
-      </c>
-      <c r="I26" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>16810326</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>deh-francisco-pinto-i</t>
+          <t>deh-gaspar-do-amaral</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Francisco Pinto</t>
+          <t>Gaspar do Amaral</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>16770527</t>
+          <t>15920000</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16080601</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>16620529</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>15</v>
+      </c>
+      <c r="G27" t="n">
+        <v>15</v>
+      </c>
+      <c r="H27" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>16810326</t>
-        </is>
-      </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16230324</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>deh-gaspar-do-amaral</t>
+          <t>deh-gaspar-ferreira</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Gaspar do Amaral</t>
+          <t>Gaspar Ferreira</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>16080601</t>
+          <t>15710000</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15890300</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>15920000</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>17</v>
+      </c>
+      <c r="G28" t="n">
+        <v>4</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>16230324</t>
-        </is>
-      </c>
-      <c r="I28" t="inlineStr"/>
+          <t>S. Bartolomeu</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>15930404</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>deh-gaspar-ferreira</t>
+          <t>deh-goncalo-alvares</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Gaspar Ferreira</t>
+          <t>Gonçalo Álvares</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>15890300</t>
+          <t>15270000</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15490101</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>15710000</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>S. Bartolomeu</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>21</v>
+      </c>
+      <c r="G29" t="n">
+        <v>19</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>15930404</t>
+          <t>Chagas</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>15680407</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>deh-goncalo-alvares</t>
+          <t>deh-inacio-pires</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Gonçalo Álvares</t>
+          <t>Inácio Pires</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15490101</t>
+          <t>17240704</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>17420427</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>15270000</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Chagas</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>17</v>
+      </c>
+      <c r="G30" t="n">
+        <v>8</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>15680407</t>
-        </is>
-      </c>
-      <c r="I30" t="inlineStr"/>
+          <t>[Para a China]</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>17500000</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>deh-inacio-pires</t>
+          <t>deh-joao-da-rocha</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Inácio Pires</t>
+          <t>João da Rocha</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>17420427</t>
+          <t>15650000</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15830000</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>17240704</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>17</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>17500000</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr"/>
+          <t>[Para a Índia]</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>15860411</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-da-rocha</t>
+          <t>deh-joao-da-silva</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>João da Rocha</t>
+          <t>João da Silva</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>15830000</t>
+          <t>16470000</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16680000</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>15650000</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>[Para a Índia]</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>15860411</t>
-        </is>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>extra_info: {"value": {"comment": "partiram nesta data os navios S. Filipe, Caranja e Jesus, Wicky n\u00e3o especifica quem foi em qual"}}</t>
-        </is>
-      </c>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>21</v>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-da-silva</t>
+          <t>deh-joao-rodrigues-de-sainan</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>João da Silva</t>
+          <t>João Rodrigues de Sainan</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>16680000</t>
+          <t>15310000</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15550000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>16470000</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>24</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Flor de la Mar</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>15560330</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-rodrigues-de-sainan</t>
+          <t>deh-joao-rodrigues-girao</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>João Rodrigues de Sainan</t>
+          <t>João Rodrigues Girão</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>15550000</t>
+          <t>15580000</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15761216</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>15310000</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Flor de la Mar</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>18</v>
+      </c>
+      <c r="G34" t="n">
+        <v>6</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>15560330</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "era novi\u00e7o"}}</t>
-        </is>
+          <t>15830408</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-rodrigues-girao</t>
+          <t>deh-joao-soeiro</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>João Rodrigues Girão</t>
+          <t>João Soeiro</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15761216</t>
+          <t>15660000</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15840000</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>15580000</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>18</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>15830408</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>15860411</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>deh-joao-soeiro</t>
+          <t>deh-jose-montanha-ii</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>João Soeiro</t>
+          <t>José Montanha</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>15840000</t>
+          <t>17080103</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>17211031</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>15660000</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>13</v>
+      </c>
+      <c r="G36" t="n">
+        <v>21</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>15860411</t>
+          <t>S. Pedro e S. Paulo</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}, "value": {"comment": "partiram nesta data os navios S. Filipe, Caranja e Jesus, Wicky n\u00e3o especifica quem foi em qual"}}</t>
-        </is>
+          <t>17420000</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>34</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>deh-jose-montanha-ii</t>
+          <t>deh-leonardo-teixeira</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>José Montanha</t>
+          <t>Leonardo Teixeira</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17211031</t>
+          <t>16700000</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16860303</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>17080103</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>S. Pedro e S. Paulo</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>15</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>17420000</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "com Monsenhor Hil\u00e1rio de Santa Rosa e tr\u00eas jesu\u00edtas destinados \u00e0 China"}}</t>
-        </is>
+          <t>16900408</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>deh-leonardo-teixeira</t>
+          <t>deh-lourenco-mexia</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Leonardo Teixeira</t>
+          <t>Lourenço Mexia</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>16860303</t>
+          <t>15390800</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15600314</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>16700000</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>20</v>
+      </c>
+      <c r="G38" t="n">
+        <v>16</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>16900408</t>
+          <t>Sta. Catarina</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}, "value": {"comment": "segundo a entrada de Cicero ter\u00e1 sido em Lisboa"}}</t>
-        </is>
+          <t>15760307</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>36</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>deh-lourenco-mexia</t>
+          <t>deh-luis-de-caldas</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Lourenço Mexia</t>
+          <t>Luís de Caldas</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>15600314</t>
+          <t>16891120</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>17041224</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>15390800</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Sta. Catarina</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>15</v>
+      </c>
+      <c r="G39" t="n">
+        <v>9</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>15760307</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "para Malaca"}}</t>
-        </is>
+          <t>17140412</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>deh-luis-de-caldas</t>
+          <t>deh-manuel-de-sa</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Luís de Caldas</t>
+          <t>Manuel de Sá</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>17041224</t>
+          <t>16580422</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16750213</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>16891120</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>16</v>
+      </c>
+      <c r="G40" t="n">
+        <v>5</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>17140412</t>
-        </is>
-      </c>
-      <c r="I40" t="inlineStr"/>
+          <t>Sto. António</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>16800404</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
@@ -2234,300 +2280,313 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>16580422</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>16750213</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>16580422</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Sto. António</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>16</v>
+      </c>
+      <c r="G41" t="n">
+        <v>34</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>16800404</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr"/>
+          <t>[Para Goa]</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>17090408</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-de-sa</t>
+          <t>deh-manuel-dias-o-novo</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Manuel de Sá</t>
+          <t>Manuel Dias, o Novo</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>16750213</t>
+          <t>15740000</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15930202</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>16580422</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>[Para Goa]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>18</v>
+      </c>
+      <c r="G42" t="n">
+        <v>8</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>17090408</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr"/>
+          <t>Santiago</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>16010411</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-dias-o-novo</t>
+          <t>deh-manuel-gaspar</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Manuel Dias, o Novo</t>
+          <t>Manuel Gaspar</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>15930202</t>
+          <t>15540000</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15750926</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>15740000</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>21</v>
+      </c>
+      <c r="G43" t="n">
+        <v>13</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>16010411</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr"/>
+          <t>S. Bernardo</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>15890404</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-gaspar</t>
+          <t>deh-manuel-jorge</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Manuel Gaspar</t>
+          <t>Manuel Jorge</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>15750926</t>
+          <t>16210000</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16380000</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>15540000</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>S. Bernardo</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>16</v>
+      </c>
+      <c r="G44" t="n">
+        <v>5</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>15890404</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr"/>
+          <t>[Para a Índia]</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>16430330</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-jorge</t>
+          <t>deh-manuel-mendes</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Manuel Jorge</t>
+          <t>Manuel Mendes</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>16380000</t>
+          <t>16560101</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16730315</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>16210000</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>[Para a Índia]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>17</v>
+      </c>
+      <c r="G45" t="n">
+        <v>7</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>16430330</t>
+          <t>Sto. António</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16800404</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-mendes</t>
+          <t>deh-manuel-osorio-i</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Manuel Mendes</t>
+          <t>Manuel Osório</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>16730315</t>
+          <t>16630305</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16780215</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>16560101</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Sto. António</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>14</v>
+      </c>
+      <c r="G46" t="n">
+        <v>8</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>16400404</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>16850000</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-osorio-i</t>
+          <t>deh-manuel-ribeiro-senior</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Manuel Osório</t>
+          <t>Manuel Ribeiro, sénior</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>16780215</t>
+          <t>16760000</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16931030</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>16630305</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>17</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>16850000</t>
+          <t>[Para a China]</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16950000</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
+        <v>18</v>
       </c>
     </row>
     <row r="48">
@@ -2543,226 +2602,221 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>16760000</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>16931030</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>16760000</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>17</v>
+      </c>
+      <c r="G48" t="n">
+        <v>3</v>
+      </c>
+      <c r="H48" t="inlineStr">
         <is>
           <t>[Para a China]</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>16950000</t>
-        </is>
-      </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "ou 16960000, n\u00e3o padre"}}</t>
-        </is>
+          <t>16960000</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>deh-manuel-ribeiro-senior</t>
+          <t>deh-mateus-de-couros</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Manuel Ribeiro, sénior</t>
+          <t>Mateus de Couros</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>16931030</t>
+          <t>15690000</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15831222</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>16760000</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>14</v>
+      </c>
+      <c r="G49" t="n">
+        <v>2</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>16960000</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "ou 16950000, n\u00e3o padre"}}</t>
-        </is>
+          <t>15860411</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>deh-mateus-de-couros</t>
+          <t>deh-matias-da-maia</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Mateus de Couros</t>
+          <t>Matias da Maia</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>15831222</t>
+          <t>16160000</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16290510</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>15690000</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>15860411</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>12</v>
+      </c>
+      <c r="G50" t="n">
+        <v>11</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Nossa Senhora da Atalaia</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>extra_info: {"type": {"comment": "partiram nesta data os navios S. Filipe, Caranja e Jesus, Wicky n\u00e3o especifica quem foi em qual", "original": "?"}, "value": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16400326</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
+        <v>23</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>deh-matias-da-maia</t>
+          <t>deh-matias-rodrigues</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Matias da Maia</t>
+          <t>Matias Rodrigues</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>16290510</t>
+          <t>16750000</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16940130</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>16160000</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Nossa Senhora da Atalaia</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>18</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>16400326</t>
+          <t>[Para a China]</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "Prisioneiro dos holandeses"}}</t>
-        </is>
+          <t>16950000</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>deh-matias-rodrigues</t>
+          <t>deh-miguel-do-amaral</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Matias Rodrigues</t>
+          <t>Miguel do Amaral</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16940130</t>
+          <t>16571213</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16770701</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>16750000</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>[Para a China]</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>19</v>
+      </c>
+      <c r="G52" t="n">
+        <v>5</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>16950000</t>
+          <t>Santiago</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}}</t>
-        </is>
+          <t>16820329</t>
+        </is>
+      </c>
+      <c r="J52" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="53">
@@ -2778,131 +2832,128 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>16571213</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>16770701</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>16571213</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>19</v>
+      </c>
+      <c r="G53" t="n">
+        <v>22</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>16820329</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>16990000</t>
+        </is>
+      </c>
+      <c r="J53" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>deh-miguel-do-amaral</t>
+          <t>deh-nicolau-pimenta</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Miguel do Amaral</t>
+          <t>Nicolau Pimenta</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>16770701</t>
+          <t>15461206</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15620502</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>16571213</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>15</v>
+      </c>
+      <c r="G54" t="n">
+        <v>34</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>16990000</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr"/>
+          <t>Conceição</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>15960410</t>
+        </is>
+      </c>
+      <c r="J54" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>deh-nicolau-pimenta</t>
+          <t>deh-pedro-de-alcacova</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Nicolau Pimenta</t>
+          <t>Pedro de Alcáçova</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>15620502</t>
+          <t>15230000</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15420000</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>15461206</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Conceição</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>15960410</t>
-        </is>
-      </c>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>19</v>
+      </c>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>deh-pedro-de-alcacova</t>
+          <t>deh-pedro-martins</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Pedro de Alcáçova</t>
+          <t>Pedro Martins</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2912,22 +2963,33 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15560525</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>15230000</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>13</v>
+      </c>
+      <c r="G56" t="n">
+        <v>29</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Santiago</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>15850413</t>
+        </is>
+      </c>
+      <c r="J56" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
@@ -2942,308 +3004,267 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>15420000</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
           <t>15560525</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>15420000</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Santiago</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>13</v>
+      </c>
+      <c r="G57" t="n">
+        <v>29</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
+          <t>Bom Jesus</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
           <t>15850413</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>deh-pedro-martins</t>
+          <t>deh-sebastiao-da-maia</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Pedro Martins</t>
+          <t>Sebastião da Maia</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>15560525</t>
+          <t>15970000</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16110000</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>15420000</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Bom Jesus</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>13</v>
+      </c>
+      <c r="G58" t="n">
+        <v>26</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr"/>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>16370406</t>
+        </is>
+      </c>
+      <c r="J58" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>deh-sebastiao-da-maia</t>
+          <t>deh-sebastiao-fernandes</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Sebastião da Maia</t>
+          <t>Sebastião Fernandes</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>16110000</t>
+          <t>15730000</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15910000</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>15970000</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>17</v>
+      </c>
+      <c r="G59" t="n">
+        <v>6</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>16370406</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr"/>
+          <t>S. Martinho</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>15970405</t>
+        </is>
+      </c>
+      <c r="J59" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>deh-sebastiao-fernandes</t>
+          <t>deh-simao-da-cunha</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Sebastião Fernandes</t>
+          <t>Simão da Cunha</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>15910000</t>
+          <t>15890000</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16060113</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>15730000</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>S. Martinho</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>16</v>
+      </c>
+      <c r="G60" t="n">
+        <v>12</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>15970405</t>
+          <t>S. Carlos</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>extra_info: {"date": {"comment": "para as \u00cdndias, ainda n\u00e3o \u00e9 padre, frade coadjutor"}}</t>
-        </is>
+          <t>16180416</t>
+        </is>
+      </c>
+      <c r="J60" t="n">
+        <v>28</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>deh-simao-da-cunha</t>
+          <t>deh-tiburcio-de-quadros</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Simão da Cunha</t>
+          <t>Tibúrcio de Quadros</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>16060113</t>
+          <t>15280000</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>15440418</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>15890000</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>S. Carlos</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>15</v>
+      </c>
+      <c r="G61" t="n">
+        <v>11</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>16180416</t>
+          <t>Sta. Marta</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"comment": "para a \u00cdndia, segundo Wicky"}}</t>
-        </is>
+          <t>15550401</t>
+        </is>
+      </c>
+      <c r="J61" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>deh-tiburcio-de-quadros</t>
+          <t>deh-tome-pereira</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Tibúrcio de Quadros</t>
+          <t>Tomé (Sancho) Pereira</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>15440418</t>
+          <t>16451101</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Coimbra</t>
+          <t>16610925</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>15280000</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Sta. Marta</t>
-        </is>
+          <t>Coimbra</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>15</v>
+      </c>
+      <c r="G62" t="n">
+        <v>5</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>15550401</t>
+          <t>?</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>extra_info: {"value": {"original": "Dehergne chama-lhe Santa Maria, corrigido a partir de Wicky"}}</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>deh-tome-pereira</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Tomé (Sancho) Pereira</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>16610925</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Coimbra</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>jesuita-entrada</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>16451101</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
           <t>16660415</t>
         </is>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>extra_info: {"date": {"comment": "n\u00e3o padre"}, "value": {"comment": "Nossa Senhora da Ajuda? vide entrada De Marini"}}</t>
-        </is>
+      <c r="J62" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update notebooks, wikidata test
</commit_message>
<xml_diff>
--- a/notebooks/jesuita-entrada-coimbra.xlsx
+++ b/notebooks/jesuita-entrada-coimbra.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,17 +476,32 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>embarque</t>
+          <t>embarque.date.year</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>embarque.date.year</t>
+          <t>age_at_embarque</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>age_at_embarque</t>
+          <t>morte.date.year</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>age_at_morte</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>mission_time</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>morte</t>
         </is>
       </c>
     </row>
@@ -527,7 +542,20 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>1579</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>56</v>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -568,16 +596,27 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Esfera</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
           <t>1551</t>
         </is>
       </c>
-      <c r="K3" t="n">
+      <c r="J3" t="n">
         <v>31</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>1571</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>52</v>
+      </c>
+      <c r="M3" t="n">
+        <v>20</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -619,16 +658,27 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>S. Filipe</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
           <t>1555</t>
         </is>
       </c>
-      <c r="K4" t="n">
+      <c r="J4" t="n">
         <v>35</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1583</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>64</v>
+      </c>
+      <c r="M4" t="n">
+        <v>28</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -670,16 +720,27 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Flor de la Mar</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
           <t>1546</t>
         </is>
       </c>
-      <c r="K5" t="n">
+      <c r="J5" t="n">
         <v>31</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>1583</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>68</v>
+      </c>
+      <c r="M5" t="n">
+        <v>36</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Negapatam</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -721,16 +782,27 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Sta. Marta</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
           <t>1555</t>
         </is>
       </c>
-      <c r="K6" t="n">
+      <c r="J6" t="n">
         <v>26</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>1572</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>44</v>
+      </c>
+      <c r="M6" t="n">
+        <v>17</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -772,16 +844,27 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Chagas</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
           <t>1568</t>
         </is>
       </c>
-      <c r="K7" t="n">
+      <c r="J7" t="n">
         <v>40</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>1573</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>46</v>
+      </c>
+      <c r="M7" t="n">
+        <v>5</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>[A caminho do Japão]</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -823,16 +906,27 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
           <t>1551</t>
         </is>
       </c>
-      <c r="K8" t="n">
+      <c r="J8" t="n">
         <v>21</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>1582</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>52</v>
+      </c>
+      <c r="M8" t="n">
+        <v>31</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -874,17 +968,16 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Flor de la Mar</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
           <t>1556</t>
         </is>
       </c>
-      <c r="K9" t="n">
+      <c r="J9" t="n">
         <v>24</v>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -925,16 +1018,27 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
           <t>1585</t>
         </is>
       </c>
-      <c r="K10" t="n">
+      <c r="J10" t="n">
         <v>42</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1598</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>55</v>
+      </c>
+      <c r="M10" t="n">
+        <v>12</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>[No mar, a caminho de Malaca]</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -976,16 +1080,27 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Sta. Catarina</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
           <t>1576</t>
         </is>
       </c>
-      <c r="K11" t="n">
+      <c r="J11" t="n">
         <v>36</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1599</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>59</v>
+      </c>
+      <c r="M11" t="n">
+        <v>23</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -1027,16 +1142,27 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Conceição</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
           <t>1596</t>
         </is>
       </c>
-      <c r="K12" t="n">
+      <c r="J12" t="n">
         <v>49</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1613</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>66</v>
+      </c>
+      <c r="M12" t="n">
+        <v>16</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Goa (Colégio Novo)</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -1078,17 +1204,16 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>S. Bernardo</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
           <t>1589</t>
         </is>
       </c>
-      <c r="K13" t="n">
+      <c r="J13" t="n">
         <v>34</v>
       </c>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1129,16 +1254,27 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
           <t>1583</t>
         </is>
       </c>
-      <c r="K14" t="n">
+      <c r="J14" t="n">
         <v>24</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1629</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>71</v>
+      </c>
+      <c r="M14" t="n">
+        <v>46</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -1180,16 +1316,27 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[Para a Índia]</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
           <t>1586</t>
         </is>
       </c>
-      <c r="K15" t="n">
+      <c r="J15" t="n">
         <v>20</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1623</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>57</v>
+      </c>
+      <c r="M15" t="n">
+        <v>36</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Hang-tcheou</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -1231,16 +1378,27 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
           <t>1586</t>
         </is>
       </c>
-      <c r="K16" t="n">
+      <c r="J16" t="n">
         <v>16</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>1632</t>
+        </is>
+      </c>
+      <c r="L16" t="n">
+        <v>63</v>
+      </c>
+      <c r="M16" t="n">
+        <v>46</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Japão</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -1282,16 +1440,27 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
           <t>1586</t>
         </is>
       </c>
-      <c r="K17" t="n">
+      <c r="J17" t="n">
         <v>19</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1607</t>
+        </is>
+      </c>
+      <c r="L17" t="n">
+        <v>41</v>
+      </c>
+      <c r="M17" t="n">
+        <v>21</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -1333,16 +1502,27 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Sto. Amaro</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
           <t>1618</t>
         </is>
       </c>
-      <c r="K18" t="n">
+      <c r="J18" t="n">
         <v>49</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1633</t>
+        </is>
+      </c>
+      <c r="L18" t="n">
+        <v>65</v>
+      </c>
+      <c r="M18" t="n">
+        <v>15</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -1384,16 +1564,27 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Nossa Senhora da Guia</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
           <t>1617</t>
         </is>
       </c>
-      <c r="K19" t="n">
+      <c r="J19" t="n">
         <v>47</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1635</t>
+        </is>
+      </c>
+      <c r="L19" t="n">
+        <v>65</v>
+      </c>
+      <c r="M19" t="n">
+        <v>17</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -1435,16 +1626,27 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
           <t>1592</t>
         </is>
       </c>
-      <c r="K20" t="n">
+      <c r="J20" t="n">
         <v>23</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1626</t>
+        </is>
+      </c>
+      <c r="L20" t="n">
+        <v>57</v>
+      </c>
+      <c r="M20" t="n">
+        <v>34</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Nagasaki</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -1486,16 +1688,27 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>S. Bartolomeu</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
           <t>1593</t>
         </is>
       </c>
-      <c r="K21" t="n">
+      <c r="J21" t="n">
         <v>21</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1649</t>
+        </is>
+      </c>
+      <c r="L21" t="n">
+        <v>78</v>
+      </c>
+      <c r="M21" t="n">
+        <v>56</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Cantão</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -1537,16 +1750,27 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>S. Martinho</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
           <t>1597</t>
         </is>
       </c>
-      <c r="K22" t="n">
+      <c r="J22" t="n">
         <v>23</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1607</t>
+        </is>
+      </c>
+      <c r="L22" t="n">
+        <v>34</v>
+      </c>
+      <c r="M22" t="n">
+        <v>10</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Japão</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -1588,16 +1812,27 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
           <t>1601</t>
         </is>
       </c>
-      <c r="K23" t="n">
+      <c r="J23" t="n">
         <v>26</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1659</t>
+        </is>
+      </c>
+      <c r="L23" t="n">
+        <v>84</v>
+      </c>
+      <c r="M23" t="n">
+        <v>57</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Hangchow</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -1639,16 +1874,27 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
           <t>1601</t>
         </is>
       </c>
-      <c r="K24" t="n">
+      <c r="J24" t="n">
         <v>21</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1614</t>
+        </is>
+      </c>
+      <c r="L24" t="n">
+        <v>34</v>
+      </c>
+      <c r="M24" t="n">
+        <v>13</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Nanquim</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -1690,16 +1936,27 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>S. Valentim</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
           <t>1600</t>
         </is>
       </c>
-      <c r="K25" t="n">
+      <c r="J25" t="n">
         <v>19</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>1634</t>
+        </is>
+      </c>
+      <c r="L25" t="n">
+        <v>53</v>
+      </c>
+      <c r="M25" t="n">
+        <v>33</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -1741,16 +1998,27 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>S. Carlos</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
           <t>1618</t>
         </is>
       </c>
-      <c r="K26" t="n">
+      <c r="J26" t="n">
         <v>28</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1660</t>
+        </is>
+      </c>
+      <c r="L26" t="n">
+        <v>71</v>
+      </c>
+      <c r="M26" t="n">
+        <v>42</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -1792,16 +2060,27 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[Para a Índia]</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
           <t>1623</t>
         </is>
       </c>
-      <c r="K27" t="n">
+      <c r="J27" t="n">
         <v>30</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>1677</t>
+        </is>
+      </c>
+      <c r="L27" t="n">
+        <v>84</v>
+      </c>
+      <c r="M27" t="n">
+        <v>53</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Foochow, Fukien</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1843,16 +2122,27 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
           <t>1623</t>
         </is>
       </c>
-      <c r="K28" t="n">
+      <c r="J28" t="n">
         <v>30</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>1646</t>
+        </is>
+      </c>
+      <c r="L28" t="n">
+        <v>53</v>
+      </c>
+      <c r="M28" t="n">
+        <v>22</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>[Perto de Hainan]</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -1894,16 +2184,27 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>S. Carlos</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
           <t>1618</t>
         </is>
       </c>
-      <c r="K29" t="n">
+      <c r="J29" t="n">
         <v>28</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>1653</t>
+        </is>
+      </c>
+      <c r="L29" t="n">
+        <v>64</v>
+      </c>
+      <c r="M29" t="n">
+        <v>35</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1945,16 +2246,27 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
           <t>1637</t>
         </is>
       </c>
-      <c r="K30" t="n">
+      <c r="J30" t="n">
         <v>39</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>1664</t>
+        </is>
+      </c>
+      <c r="L30" t="n">
+        <v>66</v>
+      </c>
+      <c r="M30" t="n">
+        <v>27</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1996,16 +2308,27 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
           <t>1634</t>
         </is>
       </c>
-      <c r="K31" t="n">
+      <c r="J31" t="n">
         <v>23</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>1677</t>
+        </is>
+      </c>
+      <c r="L31" t="n">
+        <v>66</v>
+      </c>
+      <c r="M31" t="n">
+        <v>43</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>Pequim</t>
+        </is>
       </c>
     </row>
     <row r="32">
@@ -2047,16 +2370,27 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Nossa Senhora da Atalaia</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
           <t>1640</t>
         </is>
       </c>
-      <c r="K32" t="n">
+      <c r="J32" t="n">
         <v>23</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1667</t>
+        </is>
+      </c>
+      <c r="L32" t="n">
+        <v>50</v>
+      </c>
+      <c r="M32" t="n">
+        <v>26</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Costa da Cochinchina</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -2098,17 +2432,16 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
           <t>1643</t>
         </is>
       </c>
-      <c r="K33" t="n">
+      <c r="J33" t="n">
         <v>25</v>
       </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
@@ -2149,16 +2482,27 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[Para a Índia]</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
           <t>1643</t>
         </is>
       </c>
-      <c r="K34" t="n">
+      <c r="J34" t="n">
         <v>21</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>1677</t>
+        </is>
+      </c>
+      <c r="L34" t="n">
+        <v>56</v>
+      </c>
+      <c r="M34" t="n">
+        <v>34</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>Nanquim</t>
+        </is>
       </c>
     </row>
     <row r="35">
@@ -2200,16 +2544,27 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Bom Jesus da Vidigueira</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
           <t>1657</t>
         </is>
       </c>
-      <c r="K35" t="n">
+      <c r="J35" t="n">
         <v>31</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>1661</t>
+        </is>
+      </c>
+      <c r="L35" t="n">
+        <v>36</v>
+      </c>
+      <c r="M35" t="n">
+        <v>4</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>Foochow (Fou-tcheou fou, Fukien)</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -2251,16 +2606,27 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Bom Jesus da Vidigueira</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
           <t>1657</t>
         </is>
       </c>
-      <c r="K36" t="n">
+      <c r="J36" t="n">
         <v>26</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>1657</t>
+        </is>
+      </c>
+      <c r="L36" t="n">
+        <v>27</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>[No mar, depois do Cabo da Boa Esperança]</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -2302,16 +2668,27 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
           <t>1666</t>
         </is>
       </c>
-      <c r="K37" t="n">
+      <c r="J37" t="n">
         <v>20</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>1708</t>
+        </is>
+      </c>
+      <c r="L37" t="n">
+        <v>63</v>
+      </c>
+      <c r="M37" t="n">
+        <v>42</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Pequim</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -2353,16 +2730,27 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
           <t>1694</t>
         </is>
       </c>
-      <c r="K38" t="n">
+      <c r="J38" t="n">
         <v>44</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>1709</t>
+        </is>
+      </c>
+      <c r="L38" t="n">
+        <v>58</v>
+      </c>
+      <c r="M38" t="n">
+        <v>14</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -2403,6 +2791,9 @@
       <c r="I39" t="inlineStr"/>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
@@ -2443,16 +2834,27 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
           <t>1694</t>
         </is>
       </c>
-      <c r="K40" t="n">
+      <c r="J40" t="n">
         <v>40</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>1726</t>
+        </is>
+      </c>
+      <c r="L40" t="n">
+        <v>72</v>
+      </c>
+      <c r="M40" t="n">
+        <v>31</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Nanquim</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -2494,16 +2896,27 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Sto. António</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
           <t>1680</t>
         </is>
       </c>
-      <c r="K41" t="n">
+      <c r="J41" t="n">
         <v>24</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>1741</t>
+        </is>
+      </c>
+      <c r="L41" t="n">
+        <v>84</v>
+      </c>
+      <c r="M41" t="n">
+        <v>60</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="42">
@@ -2545,16 +2958,27 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Sto. António</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
           <t>1680</t>
         </is>
       </c>
-      <c r="K42" t="n">
+      <c r="J42" t="n">
         <v>21</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>1728</t>
+        </is>
+      </c>
+      <c r="L42" t="n">
+        <v>69</v>
+      </c>
+      <c r="M42" t="n">
+        <v>48</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Lisboa</t>
+        </is>
       </c>
     </row>
     <row r="43">
@@ -2596,16 +3020,27 @@
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
           <t>1681</t>
         </is>
       </c>
-      <c r="K43" t="n">
+      <c r="J43" t="n">
         <v>18</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>1731</t>
+        </is>
+      </c>
+      <c r="L43" t="n">
+        <v>68</v>
+      </c>
+      <c r="M43" t="n">
+        <v>49</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -2647,16 +3082,27 @@
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Santiago</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
           <t>1682</t>
         </is>
       </c>
-      <c r="K44" t="n">
+      <c r="J44" t="n">
         <v>24</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>1730</t>
+        </is>
+      </c>
+      <c r="L44" t="n">
+        <v>72</v>
+      </c>
+      <c r="M44" t="n">
+        <v>48</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Coimbra</t>
+        </is>
       </c>
     </row>
     <row r="45">
@@ -2698,16 +3144,27 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
           <t>1685</t>
         </is>
       </c>
-      <c r="K45" t="n">
+      <c r="J45" t="n">
         <v>22</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>1710</t>
+        </is>
+      </c>
+      <c r="L45" t="n">
+        <v>47</v>
+      </c>
+      <c r="M45" t="n">
+        <v>25</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -2749,16 +3206,27 @@
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
           <t>1687</t>
         </is>
       </c>
-      <c r="K46" t="n">
+      <c r="J46" t="n">
         <v>20</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>1729</t>
+        </is>
+      </c>
+      <c r="L46" t="n">
+        <v>62</v>
+      </c>
+      <c r="M46" t="n">
+        <v>42</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Tonquim</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -2800,16 +3268,27 @@
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
           <t>1695</t>
         </is>
       </c>
-      <c r="K47" t="n">
+      <c r="J47" t="n">
         <v>26</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>1699</t>
+        </is>
+      </c>
+      <c r="L47" t="n">
+        <v>29</v>
+      </c>
+      <c r="M47" t="n">
+        <v>3</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Macau</t>
+        </is>
       </c>
     </row>
     <row r="48">
@@ -2851,17 +3330,16 @@
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
           <t>1690</t>
         </is>
       </c>
-      <c r="K48" t="n">
+      <c r="J48" t="n">
         <v>19</v>
       </c>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
@@ -2902,17 +3380,16 @@
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
           <t>1695</t>
         </is>
       </c>
-      <c r="K49" t="n">
+      <c r="J49" t="n">
         <v>19</v>
       </c>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
@@ -2953,16 +3430,27 @@
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
           <t>1696</t>
         </is>
       </c>
-      <c r="K50" t="n">
+      <c r="J50" t="n">
         <v>19</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>1735</t>
+        </is>
+      </c>
+      <c r="L50" t="n">
+        <v>57</v>
+      </c>
+      <c r="M50" t="n">
+        <v>38</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Pequim</t>
+        </is>
       </c>
     </row>
     <row r="51">
@@ -3004,16 +3492,27 @@
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
           <t>1694</t>
         </is>
       </c>
-      <c r="K51" t="n">
+      <c r="J51" t="n">
         <v>19</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>1721</t>
+        </is>
+      </c>
+      <c r="L51" t="n">
+        <v>46</v>
+      </c>
+      <c r="M51" t="n">
+        <v>26</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Goa</t>
+        </is>
       </c>
     </row>
     <row r="52">
@@ -3055,16 +3554,27 @@
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
           <t>1695</t>
         </is>
       </c>
-      <c r="K52" t="n">
+      <c r="J52" t="n">
         <v>18</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>1734</t>
+        </is>
+      </c>
+      <c r="L52" t="n">
+        <v>57</v>
+      </c>
+      <c r="M52" t="n">
+        <v>38</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
     </row>
     <row r="53">
@@ -3106,17 +3616,16 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
           <t>1695</t>
         </is>
       </c>
-      <c r="K53" t="n">
+      <c r="J53" t="n">
         <v>20</v>
       </c>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
@@ -3157,16 +3666,27 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>S. Francisco Xavier</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
           <t>1715</t>
         </is>
       </c>
-      <c r="K54" t="n">
+      <c r="J54" t="n">
         <v>33</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>1752</t>
+        </is>
+      </c>
+      <c r="L54" t="n">
+        <v>70</v>
+      </c>
+      <c r="M54" t="n">
+        <v>37</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -3208,17 +3728,16 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
           <t>1714</t>
         </is>
       </c>
-      <c r="K55" t="n">
+      <c r="J55" t="n">
         <v>24</v>
       </c>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
@@ -3259,16 +3778,27 @@
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>S. Pedro e S. Paulo</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
           <t>1742</t>
         </is>
       </c>
-      <c r="K56" t="n">
+      <c r="J56" t="n">
         <v>34</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>1764</t>
+        </is>
+      </c>
+      <c r="L56" t="n">
+        <v>56</v>
+      </c>
+      <c r="M56" t="n">
+        <v>22</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Castel Gandolfo</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -3310,16 +3840,27 @@
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
           <t>1727</t>
         </is>
       </c>
-      <c r="K57" t="n">
+      <c r="J57" t="n">
         <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>1751</t>
+        </is>
+      </c>
+      <c r="L57" t="n">
+        <v>44</v>
+      </c>
+      <c r="M57" t="n">
+        <v>23</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>Pequim</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -3361,16 +3902,27 @@
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>[Para a China]</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
           <t>1750</t>
         </is>
       </c>
-      <c r="K58" t="n">
+      <c r="J58" t="n">
         <v>25</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>1776</t>
+        </is>
+      </c>
+      <c r="L58" t="n">
+        <v>51</v>
+      </c>
+      <c r="M58" t="n">
+        <v>26</v>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>